<commit_message>
Implementa integração com Cloudinary
</commit_message>
<xml_diff>
--- a/static/downloads/template_importacao.xlsx
+++ b/static/downloads/template_importacao.xlsx
@@ -5,18 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Produttivo\Documents\quiz_empresa\static\downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Produttivo\Documents\quiz_empresa - Copia\static\downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8601F810-1C85-4F2A-8196-8D20367E6CA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{483F054D-57FB-45CE-91A3-5C6ED9585FDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35985" yWindow="3420" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DadosExternos_1" localSheetId="0" hidden="1">Planilha1!$A$1:$J$3</definedName>
+    <definedName name="DadosExternos_1" localSheetId="0" hidden="1">Planilha1!$A$1:$I$4</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t>tipo</t>
   </si>
@@ -60,9 +60,6 @@
     <t>tempo_limite</t>
   </si>
   <si>
-    <t>enviar_notificacao</t>
-  </si>
-  <si>
     <t>multipla_escolha</t>
   </si>
   <si>
@@ -84,9 +81,6 @@
     <t>b</t>
   </si>
   <si>
-    <t>sim</t>
-  </si>
-  <si>
     <t>verdadeiro_falso</t>
   </si>
   <si>
@@ -97,9 +91,6 @@
   </si>
   <si>
     <t/>
-  </si>
-  <si>
-    <t>não</t>
   </si>
 </sst>
 </file>
@@ -139,17 +130,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
+  <dxfs count="9">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -193,7 +182,7 @@
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="DadosExternos_1" connectionId="1" xr16:uid="{EA2BA06F-5903-4432-80BA-02CE4A714664}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="11">
-    <queryTableFields count="10">
+    <queryTableFields count="9">
       <queryTableField id="1" name="tipo" tableColumnId="11"/>
       <queryTableField id="2" name="texto" tableColumnId="2"/>
       <queryTableField id="3" name="opcao_a" tableColumnId="3"/>
@@ -203,25 +192,26 @@
       <queryTableField id="7" name="resposta_correta" tableColumnId="7"/>
       <queryTableField id="8" name="data_liberacao" tableColumnId="8"/>
       <queryTableField id="9" name="tempo_limite" tableColumnId="9"/>
-      <queryTableField id="10" name="enviar_notificacao" tableColumnId="10"/>
     </queryTableFields>
+    <queryTableDeletedFields count="1">
+      <deletedField name="enviar_notificacao"/>
+    </queryTableDeletedFields>
   </queryTableRefresh>
 </queryTable>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7701FF37-D990-418B-94AF-F7BA1546CCEA}" name="template_importacao__3" displayName="template_importacao__3" ref="A1:J3" tableType="queryTable" totalsRowShown="0">
-  <tableColumns count="10">
-    <tableColumn id="11" xr3:uid="{8DC42352-F37B-4215-827E-1EF5E687F632}" uniqueName="11" name="tipo" queryTableFieldId="1" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{D187990E-63D0-468F-A90D-749486FA9285}" uniqueName="2" name="texto" queryTableFieldId="2" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{0D8C8E6F-8EA7-4593-A961-9E5872E42AEB}" uniqueName="3" name="opcao_a" queryTableFieldId="3" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{25144922-F679-49D1-82B1-F922D4CCE334}" uniqueName="4" name="opcao_b" queryTableFieldId="4" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{BAE92546-E18A-4A02-A870-4F4DF3BDD3CC}" uniqueName="5" name="opcao_c" queryTableFieldId="5" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{03E40ADB-9E8C-4058-B2AF-D46283AE3763}" uniqueName="6" name="opcao_d" queryTableFieldId="6" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{8339EB60-8AB1-4618-BAB2-0A73FC0AF831}" uniqueName="7" name="resposta_correta" queryTableFieldId="7" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{D63087AE-D44E-4337-A6C7-82ACD0DCE10F}" uniqueName="8" name="data_liberacao" queryTableFieldId="8" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{B1464C3B-D2F7-403F-BEC4-34705F103E93}" uniqueName="9" name="tempo_limite" queryTableFieldId="9" dataDxfId="1"/>
-    <tableColumn id="10" xr3:uid="{F0A90A9B-038E-4F7A-8EB3-9D8DD43585C7}" uniqueName="10" name="enviar_notificacao" queryTableFieldId="10" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7701FF37-D990-418B-94AF-F7BA1546CCEA}" name="template_importacao__3" displayName="template_importacao__3" ref="A1:I4" tableType="queryTable" totalsRowShown="0">
+  <tableColumns count="9">
+    <tableColumn id="11" xr3:uid="{8DC42352-F37B-4215-827E-1EF5E687F632}" uniqueName="11" name="tipo" queryTableFieldId="1" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{D187990E-63D0-468F-A90D-749486FA9285}" uniqueName="2" name="texto" queryTableFieldId="2" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{0D8C8E6F-8EA7-4593-A961-9E5872E42AEB}" uniqueName="3" name="opcao_a" queryTableFieldId="3" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{25144922-F679-49D1-82B1-F922D4CCE334}" uniqueName="4" name="opcao_b" queryTableFieldId="4" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{BAE92546-E18A-4A02-A870-4F4DF3BDD3CC}" uniqueName="5" name="opcao_c" queryTableFieldId="5" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{03E40ADB-9E8C-4058-B2AF-D46283AE3763}" uniqueName="6" name="opcao_d" queryTableFieldId="6" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{8339EB60-8AB1-4618-BAB2-0A73FC0AF831}" uniqueName="7" name="resposta_correta" queryTableFieldId="7" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{D63087AE-D44E-4337-A6C7-82ACD0DCE10F}" uniqueName="8" name="data_liberacao" queryTableFieldId="8" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{B1464C3B-D2F7-403F-BEC4-34705F103E93}" uniqueName="9" name="tempo_limite" queryTableFieldId="9" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -425,10 +415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22DF1A9B-9D86-403B-8594-C7498642CF20}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -442,10 +432,9 @@
     <col min="7" max="7" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -473,31 +462,28 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>14</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>15</v>
-      </c>
-      <c r="G2" t="s">
-        <v>16</v>
       </c>
       <c r="H2" s="1">
         <v>45945</v>
@@ -505,31 +491,28 @@
       <c r="I2">
         <v>30</v>
       </c>
-      <c r="J2" t="s">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" t="s">
         <v>18</v>
-      </c>
-      <c r="B3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" t="s">
-        <v>20</v>
       </c>
       <c r="H3" s="1">
         <v>45946</v>
@@ -537,9 +520,17 @@
       <c r="I3">
         <v>20</v>
       </c>
-      <c r="J3" t="s">
-        <v>22</v>
-      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>